<commit_message>
Fix update bug caused by GitHub
</commit_message>
<xml_diff>
--- a/dev/milestones.xlsx
+++ b/dev/milestones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="174">
   <si>
     <t>Core</t>
   </si>
@@ -532,6 +532,12 @@
   </si>
   <si>
     <t>Make spawn radius more efficiently and make it removable</t>
+  </si>
+  <si>
+    <t>GitHub Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rewrite Updater and Website for GitHub </t>
   </si>
 </sst>
 </file>
@@ -685,97 +691,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="103">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -818,6 +734,96 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -848,26 +854,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -898,6 +884,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -908,16 +914,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -928,6 +924,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -948,36 +954,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -998,6 +974,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1008,36 +1024,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1078,6 +1064,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1158,46 +1154,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1208,16 +1164,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1228,6 +1174,66 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1258,16 +1264,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1278,6 +1274,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1345,6 +1351,61 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1903,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="N69" sqref="N69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3477,7 +3538,7 @@
         <v>41077</v>
       </c>
       <c r="G66" s="9" t="b">
-        <f t="shared" ref="G66:G68" si="21">ISNUMBER(F66)</f>
+        <f t="shared" ref="G66:G67" si="21">ISNUMBER(F66)</f>
         <v>1</v>
       </c>
     </row>
@@ -3507,29 +3568,34 @@
     </row>
     <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="7"/>
+      <c r="E68" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F68" s="8">
+        <v>41084</v>
+      </c>
       <c r="G68" s="9" t="b">
         <f>ISNUMBER(F68)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
-        <v>75</v>
+      <c r="A69" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>0</v>
@@ -3537,83 +3603,82 @@
       <c r="D69" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E69" s="7"/>
       <c r="G69" s="9" t="b">
-        <f t="shared" ref="G69:G75" si="22">ISNUMBER(F69)</f>
+        <f>ISNUMBER(F69)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E70" s="7"/>
       <c r="G70" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f>ISNUMBER(F70)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>99</v>
+      <c r="A71" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E71" s="7"/>
       <c r="G71" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="G71:G77" si="22">ISNUMBER(F71)</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>80</v>
+      <c r="A72" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="7"/>
       <c r="G72" s="9" t="b">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
-        <v>81</v>
+      <c r="A73" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E73" s="8"/>
+      <c r="E73" s="7"/>
       <c r="G73" s="9" t="b">
         <f t="shared" si="22"/>
         <v>0</v>
@@ -3621,10 +3686,10 @@
     </row>
     <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>27</v>
@@ -3640,10 +3705,10 @@
     </row>
     <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>27</v>
@@ -3658,225 +3723,258 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
-        <v>110</v>
+      <c r="A76" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="G76" s="9" t="b">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G76" s="9" t="b">
-        <f t="shared" ref="G76:G77" si="23">ISNUMBER(F76)</f>
+    </row>
+    <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="G77" s="9" t="b">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+    <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G77" s="9" t="b">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="7"/>
       <c r="G78" s="9" t="b">
-        <f t="shared" ref="G78" si="24">ISNUMBER(F78)</f>
+        <f>ISNUMBER(F78)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
-        <v>164</v>
+      <c r="A79" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>162</v>
+        <v>72</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="7"/>
       <c r="G79" s="9" t="b">
-        <f>ISNUMBER(F79)</f>
+        <f t="shared" ref="G79" si="23">ISNUMBER(F79)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D80" s="9"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="14"/>
+      <c r="A80" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="7"/>
       <c r="G80" s="9" t="b">
         <f>ISNUMBER(F80)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="9" t="b">
+        <f>ISNUMBER(F81)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G79">
-    <cfRule type="cellIs" dxfId="96" priority="152" operator="equal">
+  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G69:G80">
+    <cfRule type="cellIs" dxfId="102" priority="159" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="153" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="101" priority="160" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G79">
-    <cfRule type="cellIs" dxfId="94" priority="150" operator="equal">
+  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G69:G80">
+    <cfRule type="cellIs" dxfId="100" priority="157" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="93" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="131" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="125" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="98" priority="132" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="91" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="129" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="90" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="117" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="111" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="95" priority="118" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="88" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="115" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="87" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="78" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="72" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="92" priority="79" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="85" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="76" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="84" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="71" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="65" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="89" priority="72" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="82" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="69" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="81" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="60" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="54" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="86" priority="61" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="79" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="58" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G80">
-    <cfRule type="cellIs" dxfId="78" priority="37" operator="equal">
+  <conditionalFormatting sqref="G81">
+    <cfRule type="cellIs" dxfId="84" priority="44" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="38" operator="containsText" text="FALSCH">
-      <formula>NOT(ISERROR(SEARCH("FALSCH",G80)))</formula>
+    <cfRule type="containsText" dxfId="83" priority="45" operator="containsText" text="FALSCH">
+      <formula>NOT(ISERROR(SEARCH("FALSCH",G81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G80">
-    <cfRule type="cellIs" dxfId="76" priority="35" operator="equal">
+  <conditionalFormatting sqref="G81">
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="75" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="36" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="30" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="80" priority="37" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="73" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="34" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="72" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="28" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="22" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="77" priority="29" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="70" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="26" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="69" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="74" priority="23" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="67" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="20" operator="equal">
+      <formula>$C$3="Milestone"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="cellIs" dxfId="72" priority="6" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="FALSCH">
+      <formula>NOT(ISERROR(SEARCH("FALSCH",G68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3891,7 +3989,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="151" operator="containsText" id="{91E463A3-7F89-42DB-AB02-C32E69BFF8F3}">
+          <x14:cfRule type="containsText" priority="158" operator="containsText" id="{91E463A3-7F89-42DB-AB02-C32E69BFF8F3}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",A2)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -3905,10 +4003,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E78:E79 E63:E65 E70:E71 G56:G79</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="149" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
+          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E79:E80 E63:E65 E72:E73 G56:G67 G69:G80</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="156" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",A4)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -3922,10 +4020,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G79</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="147" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
+          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G69:G80</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="154" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A5)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -3939,10 +4037,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G79</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="134" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
+          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G69:G80</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="141" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E14)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -3959,7 +4057,7 @@
           <xm:sqref>E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="133" operator="containsText" id="{C684751A-87F0-471C-A31A-C3D8DB6254FF}">
+          <x14:cfRule type="containsText" priority="140" operator="containsText" id="{C684751A-87F0-471C-A31A-C3D8DB6254FF}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F14)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -3976,7 +4074,7 @@
           <xm:sqref>F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="162" operator="containsText" id="{C6B0016C-4F32-43BF-BA03-819FCC2DC4C3}">
+          <x14:cfRule type="containsText" priority="169" operator="containsText" id="{C6B0016C-4F32-43BF-BA03-819FCC2DC4C3}">
             <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C6)))</xm:f>
             <xm:f>$C$16="Milestone"</xm:f>
             <x14:dxf>
@@ -3990,10 +4088,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C78</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="123" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
+          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C79</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="130" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G21)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4010,7 +4108,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="121" operator="containsText" id="{71F5117C-34E8-484F-8A4F-16194DA252C3}">
+          <x14:cfRule type="containsText" priority="128" operator="containsText" id="{71F5117C-34E8-484F-8A4F-16194DA252C3}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G21)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4027,7 +4125,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="120" operator="containsText" id="{139CD3D0-CB09-4FF4-8D53-380F40844452}">
+          <x14:cfRule type="containsText" priority="127" operator="containsText" id="{139CD3D0-CB09-4FF4-8D53-380F40844452}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G21)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4044,7 +4142,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="119" operator="containsText" id="{3FD87057-3CA7-4AE8-9933-C50E42BB2D38}">
+          <x14:cfRule type="containsText" priority="126" operator="containsText" id="{3FD87057-3CA7-4AE8-9933-C50E42BB2D38}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E21)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4061,7 +4159,7 @@
           <xm:sqref>E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="118" operator="containsText" id="{EA545746-80D6-42D9-90B3-6B1B510D9CC3}">
+          <x14:cfRule type="containsText" priority="125" operator="containsText" id="{EA545746-80D6-42D9-90B3-6B1B510D9CC3}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F21)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4078,7 +4176,7 @@
           <xm:sqref>F21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="109" operator="containsText" id="{102BFBA1-20E5-4B5E-A799-0671076B9453}">
+          <x14:cfRule type="containsText" priority="116" operator="containsText" id="{102BFBA1-20E5-4B5E-A799-0671076B9453}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G34)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4095,7 +4193,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="107" operator="containsText" id="{680EAAAE-3B74-4D36-997E-CE1C9B9E646A}">
+          <x14:cfRule type="containsText" priority="114" operator="containsText" id="{680EAAAE-3B74-4D36-997E-CE1C9B9E646A}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G34)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4112,7 +4210,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="106" operator="containsText" id="{FDD518DD-F5D1-4C4A-977B-6C3686847040}">
+          <x14:cfRule type="containsText" priority="113" operator="containsText" id="{FDD518DD-F5D1-4C4A-977B-6C3686847040}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G34)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4129,7 +4227,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="105" operator="containsText" id="{A8C67D1C-DDBA-4CB6-8538-750623AC6FD9}">
+          <x14:cfRule type="containsText" priority="112" operator="containsText" id="{A8C67D1C-DDBA-4CB6-8538-750623AC6FD9}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E34)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4146,7 +4244,7 @@
           <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="104" operator="containsText" id="{5701881D-AC87-4402-BEA2-FCBFE1A85FBF}">
+          <x14:cfRule type="containsText" priority="111" operator="containsText" id="{5701881D-AC87-4402-BEA2-FCBFE1A85FBF}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F34)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4163,7 +4261,7 @@
           <xm:sqref>F34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="103" operator="containsText" id="{C97091A6-CD5F-4D03-94BB-3F6CDEE625C2}">
+          <x14:cfRule type="containsText" priority="110" operator="containsText" id="{C97091A6-CD5F-4D03-94BB-3F6CDEE625C2}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E22)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4180,7 +4278,7 @@
           <xm:sqref>E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="102" operator="containsText" id="{14CE30A4-7DFF-4E32-BED5-14F9E1D5BFAA}">
+          <x14:cfRule type="containsText" priority="109" operator="containsText" id="{14CE30A4-7DFF-4E32-BED5-14F9E1D5BFAA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E24)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4197,7 +4295,7 @@
           <xm:sqref>E24:E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="101" operator="containsText" id="{688E655E-E1F9-45C1-B253-8D454F96DC62}">
+          <x14:cfRule type="containsText" priority="108" operator="containsText" id="{688E655E-E1F9-45C1-B253-8D454F96DC62}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E26)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4214,7 +4312,7 @@
           <xm:sqref>E26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="100" operator="containsText" id="{405CD923-C2E4-43F2-A519-3329FA3FB5CC}">
+          <x14:cfRule type="containsText" priority="107" operator="containsText" id="{405CD923-C2E4-43F2-A519-3329FA3FB5CC}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E23)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4231,7 +4329,7 @@
           <xm:sqref>E23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="91" operator="containsText" id="{05A8CD58-D4EB-400D-B96C-B413671CB834}">
+          <x14:cfRule type="containsText" priority="98" operator="containsText" id="{05A8CD58-D4EB-400D-B96C-B413671CB834}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E47)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4248,7 +4346,7 @@
           <xm:sqref>E47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="83" operator="containsText" id="{6EA5C85B-9AA4-468A-AC6B-7E5536711992}">
+          <x14:cfRule type="containsText" priority="90" operator="containsText" id="{6EA5C85B-9AA4-468A-AC6B-7E5536711992}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E66)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4265,7 +4363,7 @@
           <xm:sqref>E66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="82" operator="containsText" id="{C6DABDAA-487A-415A-915A-6F23B11638F0}">
+          <x14:cfRule type="containsText" priority="89" operator="containsText" id="{C6DABDAA-487A-415A-915A-6F23B11638F0}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F66)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4282,8 +4380,8 @@
           <xm:sqref>F66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="81" operator="containsText" id="{494BDCB2-477F-4CCA-8E56-B54621BD2FC3}">
-            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C71)))</xm:f>
+          <x14:cfRule type="containsText" priority="88" operator="containsText" id="{494BDCB2-477F-4CCA-8E56-B54621BD2FC3}">
+            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C73)))</xm:f>
             <xm:f>$C$16="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4296,10 +4394,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C71</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="73" operator="containsText" id="{E4DC5AB8-267C-41A9-804E-ED83F72EC3B3}">
+          <xm:sqref>C73</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="80" operator="containsText" id="{E4DC5AB8-267C-41A9-804E-ED83F72EC3B3}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E37)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4316,7 +4414,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="70" operator="containsText" id="{8B21E46A-9206-438F-9A7E-A63E8282187B}">
+          <x14:cfRule type="containsText" priority="77" operator="containsText" id="{8B21E46A-9206-438F-9A7E-A63E8282187B}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G37)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4333,7 +4431,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="68" operator="containsText" id="{8F98D9E7-DDFC-4799-8534-C1508091B3F4}">
+          <x14:cfRule type="containsText" priority="75" operator="containsText" id="{8F98D9E7-DDFC-4799-8534-C1508091B3F4}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G37)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4350,7 +4448,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="67" operator="containsText" id="{AA414434-5FCB-48EB-BF6F-748F0E60759F}">
+          <x14:cfRule type="containsText" priority="74" operator="containsText" id="{AA414434-5FCB-48EB-BF6F-748F0E60759F}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G37)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4367,7 +4465,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="66" operator="containsText" id="{BA81A03D-28B6-4E80-99D2-299A88003D57}">
+          <x14:cfRule type="containsText" priority="73" operator="containsText" id="{BA81A03D-28B6-4E80-99D2-299A88003D57}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E33)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4384,7 +4482,7 @@
           <xm:sqref>E33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="63" operator="containsText" id="{3FD6F104-96C7-4A1A-AE2E-7283D0367A01}">
+          <x14:cfRule type="containsText" priority="70" operator="containsText" id="{3FD6F104-96C7-4A1A-AE2E-7283D0367A01}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G33)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4401,7 +4499,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="61" operator="containsText" id="{C7A185B6-1B1F-44D9-B7C4-2365C26DB8E6}">
+          <x14:cfRule type="containsText" priority="68" operator="containsText" id="{C7A185B6-1B1F-44D9-B7C4-2365C26DB8E6}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G33)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4418,7 +4516,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="60" operator="containsText" id="{B5321A72-B7D6-4023-A583-CB8AA2BE6BD7}">
+          <x14:cfRule type="containsText" priority="67" operator="containsText" id="{B5321A72-B7D6-4023-A583-CB8AA2BE6BD7}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G33)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4435,7 +4533,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="57" operator="containsText" id="{5A9F72EC-6BA1-4972-B137-46590E91BF3C}">
+          <x14:cfRule type="containsText" priority="64" operator="containsText" id="{5A9F72EC-6BA1-4972-B137-46590E91BF3C}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E43)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4452,7 +4550,7 @@
           <xm:sqref>E43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="55" operator="containsText" id="{B7505FED-E5A6-4248-9D59-FFC487188E7E}">
+          <x14:cfRule type="containsText" priority="62" operator="containsText" id="{B7505FED-E5A6-4248-9D59-FFC487188E7E}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E38)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4469,7 +4567,7 @@
           <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="52" operator="containsText" id="{028A3FD1-E835-4701-947E-30E08436F7E9}">
+          <x14:cfRule type="containsText" priority="59" operator="containsText" id="{028A3FD1-E835-4701-947E-30E08436F7E9}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G38)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4486,7 +4584,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="50" operator="containsText" id="{C0FF0FB4-1F1C-45F7-9171-ABEDCB571E5E}">
+          <x14:cfRule type="containsText" priority="57" operator="containsText" id="{C0FF0FB4-1F1C-45F7-9171-ABEDCB571E5E}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G38)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4503,7 +4601,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="49" operator="containsText" id="{CB24F624-94A1-45AB-84F2-E05BDB74A5FA}">
+          <x14:cfRule type="containsText" priority="56" operator="containsText" id="{CB24F624-94A1-45AB-84F2-E05BDB74A5FA}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G38)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4520,7 +4618,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="42" operator="containsText" id="{AE4A1D2A-AB1D-4F38-8BF7-D820750F29A1}">
+          <x14:cfRule type="containsText" priority="49" operator="containsText" id="{AE4A1D2A-AB1D-4F38-8BF7-D820750F29A1}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",D49)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4537,7 +4635,7 @@
           <xm:sqref>D49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{73638AB4-61D8-409D-B765-92ED92E4F8DA}">
+          <x14:cfRule type="containsText" priority="48" operator="containsText" id="{73638AB4-61D8-409D-B765-92ED92E4F8DA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E56)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4554,7 +4652,7 @@
           <xm:sqref>E56:E57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{237191AA-99D6-42EC-BDA4-43252EE012AD}">
+          <x14:cfRule type="containsText" priority="47" operator="containsText" id="{237191AA-99D6-42EC-BDA4-43252EE012AD}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E62)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4571,7 +4669,7 @@
           <xm:sqref>E62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="39" operator="containsText" id="{0FBC8BA3-30F4-429B-B067-7FA424A364D0}">
+          <x14:cfRule type="containsText" priority="46" operator="containsText" id="{0FBC8BA3-30F4-429B-B067-7FA424A364D0}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E59)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4588,8 +4686,8 @@
           <xm:sqref>E59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="36" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G80)))</xm:f>
+          <x14:cfRule type="containsText" priority="43" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G81)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4602,11 +4700,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="34" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
-            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G80)))</xm:f>
+          <xm:sqref>G81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G81)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4619,11 +4717,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A80)))</xm:f>
+          <xm:sqref>G81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A81)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4636,11 +4734,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A80:D80 G80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="32" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E80)))</xm:f>
+          <xm:sqref>A81:D81 G81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="39" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E81)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4653,11 +4751,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="31" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F80)))</xm:f>
+          <xm:sqref>E81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="38" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F81)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4670,10 +4768,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="28" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
+          <xm:sqref>F81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="35" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G50)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4690,7 +4788,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="26" operator="containsText" id="{7F37035D-B074-47C8-83DC-35EC2B7129FD}">
+          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{7F37035D-B074-47C8-83DC-35EC2B7129FD}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G50)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4707,7 +4805,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{F291EC46-F9D3-468A-9F2E-76555E389FCA}">
+          <x14:cfRule type="containsText" priority="32" operator="containsText" id="{F291EC46-F9D3-468A-9F2E-76555E389FCA}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G50)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4724,7 +4822,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{B0A63306-63FB-4869-A3A7-D2FC10025B0A}">
+          <x14:cfRule type="containsText" priority="31" operator="containsText" id="{B0A63306-63FB-4869-A3A7-D2FC10025B0A}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E50)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4741,7 +4839,7 @@
           <xm:sqref>E50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{FBBE2539-5F44-4F67-8F7B-D22340440C92}">
+          <x14:cfRule type="containsText" priority="30" operator="containsText" id="{FBBE2539-5F44-4F67-8F7B-D22340440C92}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E49)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4758,7 +4856,7 @@
           <xm:sqref>E49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{B16DF288-B2B2-4A6A-985D-3F1C228E8C8A}">
+          <x14:cfRule type="containsText" priority="27" operator="containsText" id="{B16DF288-B2B2-4A6A-985D-3F1C228E8C8A}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G48)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4775,7 +4873,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{22B41922-F462-4E8E-ADDE-A2D8E3D12D73}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{22B41922-F462-4E8E-ADDE-A2D8E3D12D73}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G48)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4792,7 +4890,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{0A028468-8270-48A0-BB36-30F8836D847E}">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{0A028468-8270-48A0-BB36-30F8836D847E}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G48)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4809,7 +4907,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{89B17EBA-11E5-4D84-A738-F43886F1E0AA}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{89B17EBA-11E5-4D84-A738-F43886F1E0AA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G52)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4826,7 +4924,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{430A5921-EF0E-4F35-96FF-D88F64E9DDC4}">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{430A5921-EF0E-4F35-96FF-D88F64E9DDC4}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G52)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4843,7 +4941,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{1442154F-A592-4E53-A6F7-935F24802789}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{1442154F-A592-4E53-A6F7-935F24802789}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G52)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4860,7 +4958,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{168A6689-AC22-47E2-B1C6-FD4463744077}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{168A6689-AC22-47E2-B1C6-FD4463744077}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E58)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4877,7 +4975,7 @@
           <xm:sqref>E58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{54B74BD1-7DC1-430F-8655-47AA7D79B3D0}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{54B74BD1-7DC1-430F-8655-47AA7D79B3D0}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E60)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4894,8 +4992,8 @@
           <xm:sqref>E60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{4C3F2991-D8EC-410C-9B0B-CF4EC4549A8D}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E69)))</xm:f>
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{4C3F2991-D8EC-410C-9B0B-CF4EC4549A8D}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E71)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4908,10 +5006,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E69</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{B92B02FA-3804-4C2D-8DFB-01196540492A}">
+          <xm:sqref>E71</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{B92B02FA-3804-4C2D-8DFB-01196540492A}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E61)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4928,7 +5026,7 @@
           <xm:sqref>E61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{45D97C8C-545E-48ED-A7DC-48EB679DFF23}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{45D97C8C-545E-48ED-A7DC-48EB679DFF23}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E48)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4945,7 +5043,7 @@
           <xm:sqref>E48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{250802EA-0165-4C33-8BF4-B9BD39D14E27}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{250802EA-0165-4C33-8BF4-B9BD39D14E27}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E51)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4962,7 +5060,7 @@
           <xm:sqref>E51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{6F8E8C81-37C7-456F-AB40-6BB37581870D}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{6F8E8C81-37C7-456F-AB40-6BB37581870D}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E52)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4979,7 +5077,92 @@
           <xm:sqref>E52:E55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{7B8D20FF-1BC4-43A8-A3FB-313BCF9C61D9}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{7B8D20FF-1BC4-43A8-A3FB-313BCF9C61D9}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E70)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E70</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{4D7DB7FF-0A08-48FF-88DA-DD1F0BCC6135}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E67)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{74FFE708-7A19-4167-8496-5B905FC265E4}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G68)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AF0A3521-EB4E-400D-844A-5B92C927A411}">
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G68)))</xm:f>
+            <xm:f>$C$4="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{33FCAECE-C126-4CD8-88BB-BA2CCA64EE6E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G68)))</xm:f>
+            <xm:f>$C$7="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A476B2B1-08FD-4830-9685-2B9301ABC130}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E68)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4994,23 +5177,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>E68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{4D7DB7FF-0A08-48FF-88DA-DD1F0BCC6135}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E67)))</xm:f>
-            <xm:f>$C$2="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E67</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Language keys have been completed
- New language keys have been added (en, de)
- A few gameplay bugs have been resolved
</commit_message>
<xml_diff>
--- a/dev/milestones.xlsx
+++ b/dev/milestones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="178">
   <si>
     <t>Core</t>
   </si>
@@ -255,18 +255,12 @@
     <t>Gameplay</t>
   </si>
   <si>
-    <t>Create a first worldmap</t>
-  </si>
-  <si>
     <t>Design - Worlds</t>
   </si>
   <si>
     <t>Design - Creatures</t>
   </si>
   <si>
-    <t>Create for each fraction 5 units</t>
-  </si>
-  <si>
     <t>Design - Maps</t>
   </si>
   <si>
@@ -544,6 +538,18 @@
   </si>
   <si>
     <t>Create a file scanner in order to scan the file structure</t>
+  </si>
+  <si>
+    <t>Create first 2 units</t>
+  </si>
+  <si>
+    <t>Create 3 first worldmaps</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Complete all language keys</t>
   </si>
 </sst>
 </file>
@@ -2035,10 +2041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2670,7 +2676,7 @@
         <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>30</v>
@@ -2694,7 +2700,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>30</v>
@@ -2715,10 +2721,10 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>30</v>
@@ -2739,10 +2745,10 @@
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>0</v>
@@ -2763,10 +2769,10 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>30</v>
@@ -2787,13 +2793,13 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>21</v>
@@ -2811,10 +2817,10 @@
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>30</v>
@@ -2855,10 +2861,10 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>0</v>
@@ -2879,10 +2885,10 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>0</v>
@@ -2903,10 +2909,10 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>30</v>
@@ -2927,10 +2933,10 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>30</v>
@@ -2954,7 +2960,7 @@
         <v>57</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>72</v>
@@ -2975,10 +2981,10 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>78</v>
@@ -2999,10 +3005,10 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>0</v>
@@ -3023,10 +3029,10 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>30</v>
@@ -3071,10 +3077,10 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>78</v>
@@ -3095,10 +3101,10 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>30</v>
@@ -3119,10 +3125,10 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>67</v>
@@ -3163,10 +3169,10 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>0</v>
@@ -3187,13 +3193,13 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>8</v>
@@ -3211,10 +3217,10 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>0</v>
@@ -3235,10 +3241,10 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>30</v>
@@ -3259,10 +3265,10 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>0</v>
@@ -3283,10 +3289,10 @@
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>0</v>
@@ -3307,10 +3313,10 @@
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>78</v>
@@ -3331,10 +3337,10 @@
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>0</v>
@@ -3355,10 +3361,10 @@
     </row>
     <row r="56" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>0</v>
@@ -3379,10 +3385,10 @@
     </row>
     <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>0</v>
@@ -3403,10 +3409,10 @@
     </row>
     <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>30</v>
@@ -3427,10 +3433,10 @@
     </row>
     <row r="59" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>34</v>
@@ -3451,10 +3457,10 @@
     </row>
     <row r="60" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>78</v>
@@ -3499,10 +3505,10 @@
     </row>
     <row r="62" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>30</v>
@@ -3523,13 +3529,13 @@
     </row>
     <row r="63" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>8</v>
@@ -3547,13 +3553,13 @@
     </row>
     <row r="64" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>8</v>
@@ -3571,10 +3577,10 @@
     </row>
     <row r="65" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>78</v>
@@ -3595,7 +3601,7 @@
     </row>
     <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>17</v>
@@ -3615,10 +3621,10 @@
     </row>
     <row r="67" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>78</v>
@@ -3639,10 +3645,10 @@
     </row>
     <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>0</v>
@@ -3663,10 +3669,10 @@
     </row>
     <row r="69" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>0</v>
@@ -3687,10 +3693,10 @@
     </row>
     <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>111</v>
+        <v>177</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>0</v>
@@ -3698,17 +3704,23 @@
       <c r="D70" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="E70" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="8">
+        <v>41087</v>
+      </c>
       <c r="G70" s="9" t="b">
         <f>ISNUMBER(F70)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>78</v>
@@ -3743,10 +3755,10 @@
     </row>
     <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>30</v>
@@ -3762,10 +3774,10 @@
     </row>
     <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>72</v>
@@ -3781,10 +3793,10 @@
     </row>
     <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>79</v>
+        <v>175</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>27</v>
@@ -3800,10 +3812,10 @@
     </row>
     <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>27</v>
@@ -3819,10 +3831,10 @@
     </row>
     <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>27</v>
@@ -3838,10 +3850,10 @@
     </row>
     <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>27</v>
@@ -3856,81 +3868,99 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
-        <v>112</v>
+      <c r="A79" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="E79" s="7"/>
       <c r="G79" s="9" t="b">
-        <f>ISNUMBER(F79)</f>
+        <f t="shared" ref="G79" si="23">ISNUMBER(F79)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
-        <v>70</v>
+      <c r="A80" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="7"/>
       <c r="G80" s="9" t="b">
-        <f t="shared" ref="G80" si="23">ISNUMBER(F80)</f>
+        <f>ISNUMBER(F80)</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="7"/>
+      <c r="A81" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="9" t="b">
         <f>ISNUMBER(F81)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="14"/>
+      <c r="A82" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="G82" s="9" t="b">
         <f>ISNUMBER(F82)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="83" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="9" t="b">
+        <f>ISNUMBER(F83)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G70:G81">
+  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G71:G80 G82:G83">
     <cfRule type="cellIs" dxfId="109" priority="159" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -3938,7 +3968,7 @@
       <formula>NOT(ISERROR(SEARCH("FALSCH",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G70:G81">
+  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G71:G80 G82:G83">
     <cfRule type="cellIs" dxfId="107" priority="157" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
@@ -4008,15 +4038,15 @@
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
+  <conditionalFormatting sqref="G81">
     <cfRule type="cellIs" dxfId="91" priority="44" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="90" priority="45" operator="containsText" text="FALSCH">
-      <formula>NOT(ISERROR(SEARCH("FALSCH",G82)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSCH",G81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
+  <conditionalFormatting sqref="G81">
     <cfRule type="cellIs" dxfId="89" priority="42" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
@@ -4060,7 +4090,7 @@
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G69">
+  <conditionalFormatting sqref="G68:G70">
     <cfRule type="cellIs" dxfId="79" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4068,7 +4098,7 @@
       <formula>NOT(ISERROR(SEARCH("FALSCH",G68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G69">
+  <conditionalFormatting sqref="G68:G70">
     <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
@@ -4098,7 +4128,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E80:E81 E63:E65 E73:E74 G56:G67 G70:G81</xm:sqref>
+          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E79:E80 E63:E65 E73:E74 G56:G67 G71:G80 G82:G83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="156" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
@@ -4115,7 +4145,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G70:G81</xm:sqref>
+          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G71:G80 G82:G83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="154" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
@@ -4132,7 +4162,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G70:G81</xm:sqref>
+          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G71:G80 G82:G83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="141" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
@@ -4183,7 +4213,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C80</xm:sqref>
+          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C79</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="130" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
@@ -4782,7 +4812,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="43" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G82)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G81)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4795,11 +4825,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G82</xm:sqref>
+          <xm:sqref>G81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="41" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
-            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G82)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G81)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4812,11 +4842,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G82</xm:sqref>
+          <xm:sqref>G81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="40" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A82)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A81)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4829,11 +4859,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A82:D82 G82</xm:sqref>
+          <xm:sqref>A81:D81 G81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="39" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E82)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E81)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4846,11 +4876,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E82</xm:sqref>
+          <xm:sqref>E81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="38" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F82)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F81)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4863,7 +4893,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F82</xm:sqref>
+          <xm:sqref>F81</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="35" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
@@ -5220,7 +5250,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G69</xm:sqref>
+          <xm:sqref>G68:G70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AF0A3521-EB4E-400D-844A-5B92C927A411}">
@@ -5237,7 +5267,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G69</xm:sqref>
+          <xm:sqref>G68:G70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{33FCAECE-C126-4CD8-88BB-BA2CCA64EE6E}">
@@ -5254,7 +5284,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G69</xm:sqref>
+          <xm:sqref>G68:G70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A476B2B1-08FD-4830-9685-2B9301ABC130}">
@@ -5271,7 +5301,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E68:E69</xm:sqref>
+          <xm:sqref>E68:E70</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Test animations have been implemented
</commit_message>
<xml_diff>
--- a/dev/milestones.xlsx
+++ b/dev/milestones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
   <si>
     <t>Core</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t>Implement logic to win the game</t>
+  </si>
+  <si>
+    <t>Popup Menu Bug</t>
+  </si>
+  <si>
+    <t>Fade Popup out when specific object isn't active</t>
   </si>
 </sst>
 </file>
@@ -709,17 +715,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="113">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -772,6 +768,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2047,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3747,70 +3783,72 @@
     </row>
     <row r="72" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="7"/>
+      <c r="E72" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G72" s="9" t="b">
         <f>ISNUMBER(F72)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
-        <v>75</v>
+      <c r="A73" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="7"/>
       <c r="G73" s="9" t="b">
-        <f t="shared" ref="G73:G79" si="22">ISNUMBER(F73)</f>
+        <f>ISNUMBER(F73)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
-        <v>90</v>
+      <c r="A74" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E74" s="7"/>
       <c r="G74" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="G74:G80" si="22">ISNUMBER(F74)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>21</v>
@@ -3822,19 +3860,19 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
-        <v>79</v>
+      <c r="A76" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="7"/>
       <c r="G76" s="9" t="b">
         <f t="shared" si="22"/>
         <v>0</v>
@@ -3842,10 +3880,10 @@
     </row>
     <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>27</v>
@@ -3861,10 +3899,10 @@
     </row>
     <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>27</v>
@@ -3880,10 +3918,10 @@
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>27</v>
@@ -3899,73 +3937,74 @@
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="8"/>
+      <c r="G80" s="9" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="7"/>
-      <c r="G80" s="9" t="b">
-        <f t="shared" ref="G80" si="23">ISNUMBER(F80)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="7"/>
       <c r="G81" s="9" t="b">
-        <f>ISNUMBER(F81)</f>
+        <f t="shared" ref="G81" si="23">ISNUMBER(F81)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="14"/>
+      <c r="A82" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="7"/>
       <c r="G82" s="9" t="b">
         <f>ISNUMBER(F82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A83" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="9"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="9" t="b">
         <f>ISNUMBER(F83)</f>
         <v>0</v>
@@ -3973,10 +4012,10 @@
     </row>
     <row r="84" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>0</v>
@@ -3989,147 +4028,165 @@
         <v>0</v>
       </c>
     </row>
+    <row r="85" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="9" t="b">
+        <f>ISNUMBER(F85)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G72:G81 G83:G84">
-    <cfRule type="cellIs" dxfId="109" priority="159" operator="equal">
+  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85">
+    <cfRule type="cellIs" dxfId="112" priority="161" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="160" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="111" priority="162" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G72:G81 G83:G84">
-    <cfRule type="cellIs" dxfId="107" priority="157" operator="equal">
+  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85">
+    <cfRule type="cellIs" dxfId="110" priority="159" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="106" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="133" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="132" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="108" priority="134" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="104" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="131" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="103" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="118" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="105" priority="120" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="101" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="117" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="100" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="80" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="79" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="102" priority="81" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="98" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="78" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="97" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="73" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="72" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="99" priority="74" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="95" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="71" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="94" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="62" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="61" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="96" priority="63" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="92" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="60" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="cellIs" dxfId="91" priority="44" operator="equal">
+  <conditionalFormatting sqref="G83">
+    <cfRule type="cellIs" dxfId="94" priority="46" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="45" operator="containsText" text="FALSCH">
-      <formula>NOT(ISERROR(SEARCH("FALSCH",G82)))</formula>
+    <cfRule type="containsText" dxfId="93" priority="47" operator="containsText" text="FALSCH">
+      <formula>NOT(ISERROR(SEARCH("FALSCH",G83)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="cellIs" dxfId="89" priority="42" operator="equal">
+  <conditionalFormatting sqref="G83">
+    <cfRule type="cellIs" dxfId="92" priority="44" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="88" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="38" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="90" priority="39" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="86" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="36" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="85" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="29" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="87" priority="31" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="83" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="28" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="23" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="84" priority="25" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="80" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="22" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G71">
-    <cfRule type="cellIs" dxfId="79" priority="6" operator="equal">
+  <conditionalFormatting sqref="G68:G72">
+    <cfRule type="cellIs" dxfId="82" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="7" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G71">
-    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+  <conditionalFormatting sqref="G68:G72">
+    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4144,7 +4201,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="158" operator="containsText" id="{91E463A3-7F89-42DB-AB02-C32E69BFF8F3}">
+          <x14:cfRule type="containsText" priority="160" operator="containsText" id="{91E463A3-7F89-42DB-AB02-C32E69BFF8F3}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",A2)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4158,10 +4215,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E80:E81 E63:E65 E74:E75 G56:G67 G72:G81 G83:G84</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="156" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
+          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E81:E82 E63:E65 E75:E76 G56:G67 G73:G82 G84:G85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="158" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",A4)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4175,10 +4232,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G72:G81 G83:G84</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="154" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
+          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="156" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A5)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4192,10 +4249,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G72:G81 G83:G84</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="141" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
+          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G73:G82 G84:G85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="143" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E14)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4212,7 +4269,7 @@
           <xm:sqref>E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="140" operator="containsText" id="{C684751A-87F0-471C-A31A-C3D8DB6254FF}">
+          <x14:cfRule type="containsText" priority="142" operator="containsText" id="{C684751A-87F0-471C-A31A-C3D8DB6254FF}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F14)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4229,7 +4286,7 @@
           <xm:sqref>F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="169" operator="containsText" id="{C6B0016C-4F32-43BF-BA03-819FCC2DC4C3}">
+          <x14:cfRule type="containsText" priority="171" operator="containsText" id="{C6B0016C-4F32-43BF-BA03-819FCC2DC4C3}">
             <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C6)))</xm:f>
             <xm:f>$C$16="Milestone"</xm:f>
             <x14:dxf>
@@ -4243,10 +4300,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C80</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="130" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
+          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="132" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G21)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4263,7 +4320,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="128" operator="containsText" id="{71F5117C-34E8-484F-8A4F-16194DA252C3}">
+          <x14:cfRule type="containsText" priority="130" operator="containsText" id="{71F5117C-34E8-484F-8A4F-16194DA252C3}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G21)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4280,7 +4337,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="127" operator="containsText" id="{139CD3D0-CB09-4FF4-8D53-380F40844452}">
+          <x14:cfRule type="containsText" priority="129" operator="containsText" id="{139CD3D0-CB09-4FF4-8D53-380F40844452}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G21)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4297,7 +4354,7 @@
           <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="126" operator="containsText" id="{3FD87057-3CA7-4AE8-9933-C50E42BB2D38}">
+          <x14:cfRule type="containsText" priority="128" operator="containsText" id="{3FD87057-3CA7-4AE8-9933-C50E42BB2D38}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E21)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4314,7 +4371,7 @@
           <xm:sqref>E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="125" operator="containsText" id="{EA545746-80D6-42D9-90B3-6B1B510D9CC3}">
+          <x14:cfRule type="containsText" priority="127" operator="containsText" id="{EA545746-80D6-42D9-90B3-6B1B510D9CC3}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F21)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4331,7 +4388,7 @@
           <xm:sqref>F21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="116" operator="containsText" id="{102BFBA1-20E5-4B5E-A799-0671076B9453}">
+          <x14:cfRule type="containsText" priority="118" operator="containsText" id="{102BFBA1-20E5-4B5E-A799-0671076B9453}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G34)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4348,7 +4405,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="114" operator="containsText" id="{680EAAAE-3B74-4D36-997E-CE1C9B9E646A}">
+          <x14:cfRule type="containsText" priority="116" operator="containsText" id="{680EAAAE-3B74-4D36-997E-CE1C9B9E646A}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G34)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4365,7 +4422,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="113" operator="containsText" id="{FDD518DD-F5D1-4C4A-977B-6C3686847040}">
+          <x14:cfRule type="containsText" priority="115" operator="containsText" id="{FDD518DD-F5D1-4C4A-977B-6C3686847040}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G34)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4382,7 +4439,7 @@
           <xm:sqref>G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="112" operator="containsText" id="{A8C67D1C-DDBA-4CB6-8538-750623AC6FD9}">
+          <x14:cfRule type="containsText" priority="114" operator="containsText" id="{A8C67D1C-DDBA-4CB6-8538-750623AC6FD9}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E34)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4399,7 +4456,7 @@
           <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="111" operator="containsText" id="{5701881D-AC87-4402-BEA2-FCBFE1A85FBF}">
+          <x14:cfRule type="containsText" priority="113" operator="containsText" id="{5701881D-AC87-4402-BEA2-FCBFE1A85FBF}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F34)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4416,7 +4473,7 @@
           <xm:sqref>F34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="110" operator="containsText" id="{C97091A6-CD5F-4D03-94BB-3F6CDEE625C2}">
+          <x14:cfRule type="containsText" priority="112" operator="containsText" id="{C97091A6-CD5F-4D03-94BB-3F6CDEE625C2}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E22)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4433,7 +4490,7 @@
           <xm:sqref>E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="109" operator="containsText" id="{14CE30A4-7DFF-4E32-BED5-14F9E1D5BFAA}">
+          <x14:cfRule type="containsText" priority="111" operator="containsText" id="{14CE30A4-7DFF-4E32-BED5-14F9E1D5BFAA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E24)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4450,7 +4507,7 @@
           <xm:sqref>E24:E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="108" operator="containsText" id="{688E655E-E1F9-45C1-B253-8D454F96DC62}">
+          <x14:cfRule type="containsText" priority="110" operator="containsText" id="{688E655E-E1F9-45C1-B253-8D454F96DC62}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E26)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4467,7 +4524,7 @@
           <xm:sqref>E26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="107" operator="containsText" id="{405CD923-C2E4-43F2-A519-3329FA3FB5CC}">
+          <x14:cfRule type="containsText" priority="109" operator="containsText" id="{405CD923-C2E4-43F2-A519-3329FA3FB5CC}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E23)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4484,7 +4541,7 @@
           <xm:sqref>E23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="98" operator="containsText" id="{05A8CD58-D4EB-400D-B96C-B413671CB834}">
+          <x14:cfRule type="containsText" priority="100" operator="containsText" id="{05A8CD58-D4EB-400D-B96C-B413671CB834}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E47)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4501,7 +4558,7 @@
           <xm:sqref>E47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="90" operator="containsText" id="{6EA5C85B-9AA4-468A-AC6B-7E5536711992}">
+          <x14:cfRule type="containsText" priority="92" operator="containsText" id="{6EA5C85B-9AA4-468A-AC6B-7E5536711992}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E66)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4518,7 +4575,7 @@
           <xm:sqref>E66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="89" operator="containsText" id="{C6DABDAA-487A-415A-915A-6F23B11638F0}">
+          <x14:cfRule type="containsText" priority="91" operator="containsText" id="{C6DABDAA-487A-415A-915A-6F23B11638F0}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F66)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4535,8 +4592,8 @@
           <xm:sqref>F66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="88" operator="containsText" id="{494BDCB2-477F-4CCA-8E56-B54621BD2FC3}">
-            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C75)))</xm:f>
+          <x14:cfRule type="containsText" priority="90" operator="containsText" id="{494BDCB2-477F-4CCA-8E56-B54621BD2FC3}">
+            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C76)))</xm:f>
             <xm:f>$C$16="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4549,10 +4606,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C75</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="80" operator="containsText" id="{E4DC5AB8-267C-41A9-804E-ED83F72EC3B3}">
+          <xm:sqref>C76</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="82" operator="containsText" id="{E4DC5AB8-267C-41A9-804E-ED83F72EC3B3}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E37)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4569,7 +4626,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="77" operator="containsText" id="{8B21E46A-9206-438F-9A7E-A63E8282187B}">
+          <x14:cfRule type="containsText" priority="79" operator="containsText" id="{8B21E46A-9206-438F-9A7E-A63E8282187B}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G37)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4586,7 +4643,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="75" operator="containsText" id="{8F98D9E7-DDFC-4799-8534-C1508091B3F4}">
+          <x14:cfRule type="containsText" priority="77" operator="containsText" id="{8F98D9E7-DDFC-4799-8534-C1508091B3F4}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G37)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4603,7 +4660,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="74" operator="containsText" id="{AA414434-5FCB-48EB-BF6F-748F0E60759F}">
+          <x14:cfRule type="containsText" priority="76" operator="containsText" id="{AA414434-5FCB-48EB-BF6F-748F0E60759F}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G37)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4620,7 +4677,7 @@
           <xm:sqref>G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="73" operator="containsText" id="{BA81A03D-28B6-4E80-99D2-299A88003D57}">
+          <x14:cfRule type="containsText" priority="75" operator="containsText" id="{BA81A03D-28B6-4E80-99D2-299A88003D57}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E33)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4637,7 +4694,7 @@
           <xm:sqref>E33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="70" operator="containsText" id="{3FD6F104-96C7-4A1A-AE2E-7283D0367A01}">
+          <x14:cfRule type="containsText" priority="72" operator="containsText" id="{3FD6F104-96C7-4A1A-AE2E-7283D0367A01}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G33)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4654,7 +4711,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="68" operator="containsText" id="{C7A185B6-1B1F-44D9-B7C4-2365C26DB8E6}">
+          <x14:cfRule type="containsText" priority="70" operator="containsText" id="{C7A185B6-1B1F-44D9-B7C4-2365C26DB8E6}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G33)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4671,7 +4728,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="67" operator="containsText" id="{B5321A72-B7D6-4023-A583-CB8AA2BE6BD7}">
+          <x14:cfRule type="containsText" priority="69" operator="containsText" id="{B5321A72-B7D6-4023-A583-CB8AA2BE6BD7}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G33)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4688,7 +4745,7 @@
           <xm:sqref>G33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="64" operator="containsText" id="{5A9F72EC-6BA1-4972-B137-46590E91BF3C}">
+          <x14:cfRule type="containsText" priority="66" operator="containsText" id="{5A9F72EC-6BA1-4972-B137-46590E91BF3C}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E43)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4705,7 +4762,7 @@
           <xm:sqref>E43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="62" operator="containsText" id="{B7505FED-E5A6-4248-9D59-FFC487188E7E}">
+          <x14:cfRule type="containsText" priority="64" operator="containsText" id="{B7505FED-E5A6-4248-9D59-FFC487188E7E}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E38)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4722,7 +4779,7 @@
           <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="59" operator="containsText" id="{028A3FD1-E835-4701-947E-30E08436F7E9}">
+          <x14:cfRule type="containsText" priority="61" operator="containsText" id="{028A3FD1-E835-4701-947E-30E08436F7E9}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G38)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4739,7 +4796,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="57" operator="containsText" id="{C0FF0FB4-1F1C-45F7-9171-ABEDCB571E5E}">
+          <x14:cfRule type="containsText" priority="59" operator="containsText" id="{C0FF0FB4-1F1C-45F7-9171-ABEDCB571E5E}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G38)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4756,7 +4813,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="56" operator="containsText" id="{CB24F624-94A1-45AB-84F2-E05BDB74A5FA}">
+          <x14:cfRule type="containsText" priority="58" operator="containsText" id="{CB24F624-94A1-45AB-84F2-E05BDB74A5FA}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G38)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4773,7 +4830,7 @@
           <xm:sqref>G38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="49" operator="containsText" id="{AE4A1D2A-AB1D-4F38-8BF7-D820750F29A1}">
+          <x14:cfRule type="containsText" priority="51" operator="containsText" id="{AE4A1D2A-AB1D-4F38-8BF7-D820750F29A1}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",D49)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4790,7 +4847,7 @@
           <xm:sqref>D49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="48" operator="containsText" id="{73638AB4-61D8-409D-B765-92ED92E4F8DA}">
+          <x14:cfRule type="containsText" priority="50" operator="containsText" id="{73638AB4-61D8-409D-B765-92ED92E4F8DA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E56)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4807,7 +4864,7 @@
           <xm:sqref>E56:E57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="47" operator="containsText" id="{237191AA-99D6-42EC-BDA4-43252EE012AD}">
+          <x14:cfRule type="containsText" priority="49" operator="containsText" id="{237191AA-99D6-42EC-BDA4-43252EE012AD}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E62)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4824,7 +4881,7 @@
           <xm:sqref>E62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="46" operator="containsText" id="{0FBC8BA3-30F4-429B-B067-7FA424A364D0}">
+          <x14:cfRule type="containsText" priority="48" operator="containsText" id="{0FBC8BA3-30F4-429B-B067-7FA424A364D0}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E59)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4841,8 +4898,8 @@
           <xm:sqref>E59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="43" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G82)))</xm:f>
+          <x14:cfRule type="containsText" priority="45" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G83)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4855,11 +4912,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G82</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
-            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G82)))</xm:f>
+          <xm:sqref>G83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="43" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G83)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4872,11 +4929,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G82</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A82)))</xm:f>
+          <xm:sqref>G83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="42" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A83)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4889,11 +4946,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A82:D82 G82</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="39" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E82)))</xm:f>
+          <xm:sqref>A83:D83 G83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E83)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4906,11 +4963,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E82</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="38" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F82)))</xm:f>
+          <xm:sqref>E83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F83)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4923,10 +4980,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F82</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="35" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
+          <xm:sqref>F83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="37" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G50)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4943,7 +5000,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{7F37035D-B074-47C8-83DC-35EC2B7129FD}">
+          <x14:cfRule type="containsText" priority="35" operator="containsText" id="{7F37035D-B074-47C8-83DC-35EC2B7129FD}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G50)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -4960,7 +5017,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="32" operator="containsText" id="{F291EC46-F9D3-468A-9F2E-76555E389FCA}">
+          <x14:cfRule type="containsText" priority="34" operator="containsText" id="{F291EC46-F9D3-468A-9F2E-76555E389FCA}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G50)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -4977,7 +5034,7 @@
           <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="31" operator="containsText" id="{B0A63306-63FB-4869-A3A7-D2FC10025B0A}">
+          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{B0A63306-63FB-4869-A3A7-D2FC10025B0A}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E50)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -4994,7 +5051,7 @@
           <xm:sqref>E50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="30" operator="containsText" id="{FBBE2539-5F44-4F67-8F7B-D22340440C92}">
+          <x14:cfRule type="containsText" priority="32" operator="containsText" id="{FBBE2539-5F44-4F67-8F7B-D22340440C92}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E49)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5011,7 +5068,7 @@
           <xm:sqref>E49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="27" operator="containsText" id="{B16DF288-B2B2-4A6A-985D-3F1C228E8C8A}">
+          <x14:cfRule type="containsText" priority="29" operator="containsText" id="{B16DF288-B2B2-4A6A-985D-3F1C228E8C8A}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G48)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5028,7 +5085,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{22B41922-F462-4E8E-ADDE-A2D8E3D12D73}">
+          <x14:cfRule type="containsText" priority="27" operator="containsText" id="{22B41922-F462-4E8E-ADDE-A2D8E3D12D73}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G48)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -5045,7 +5102,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{0A028468-8270-48A0-BB36-30F8836D847E}">
+          <x14:cfRule type="containsText" priority="26" operator="containsText" id="{0A028468-8270-48A0-BB36-30F8836D847E}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G48)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -5062,7 +5119,7 @@
           <xm:sqref>G48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{89B17EBA-11E5-4D84-A738-F43886F1E0AA}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{89B17EBA-11E5-4D84-A738-F43886F1E0AA}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G52)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5079,7 +5136,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{430A5921-EF0E-4F35-96FF-D88F64E9DDC4}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{430A5921-EF0E-4F35-96FF-D88F64E9DDC4}">
             <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G52)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
@@ -5096,7 +5153,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{1442154F-A592-4E53-A6F7-935F24802789}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{1442154F-A592-4E53-A6F7-935F24802789}">
             <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G52)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
@@ -5113,7 +5170,7 @@
           <xm:sqref>G52:G55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{168A6689-AC22-47E2-B1C6-FD4463744077}">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{168A6689-AC22-47E2-B1C6-FD4463744077}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E58)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5130,7 +5187,7 @@
           <xm:sqref>E58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{54B74BD1-7DC1-430F-8655-47AA7D79B3D0}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{54B74BD1-7DC1-430F-8655-47AA7D79B3D0}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E60)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5147,7 +5204,92 @@
           <xm:sqref>E60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{4C3F2991-D8EC-410C-9B0B-CF4EC4549A8D}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{4C3F2991-D8EC-410C-9B0B-CF4EC4549A8D}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E74)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E74</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{B92B02FA-3804-4C2D-8DFB-01196540492A}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E61)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{45D97C8C-545E-48ED-A7DC-48EB679DFF23}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E48)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{250802EA-0165-4C33-8BF4-B9BD39D14E27}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E51)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E51</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{6F8E8C81-37C7-456F-AB40-6BB37581870D}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E52)))</xm:f>
+            <xm:f>$C$2="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E52:E55</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{7B8D20FF-1BC4-43A8-A3FB-313BCF9C61D9}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E73)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5164,8 +5306,8 @@
           <xm:sqref>E73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{B92B02FA-3804-4C2D-8DFB-01196540492A}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E61)))</xm:f>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{4D7DB7FF-0A08-48FF-88DA-DD1F0BCC6135}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E67)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -5178,11 +5320,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E61</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{45D97C8C-545E-48ED-A7DC-48EB679DFF23}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E48)))</xm:f>
+          <xm:sqref>E67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{74FFE708-7A19-4167-8496-5B905FC265E4}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G68)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -5195,11 +5337,45 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{250802EA-0165-4C33-8BF4-B9BD39D14E27}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E51)))</xm:f>
+          <xm:sqref>G68:G72</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{AF0A3521-EB4E-400D-844A-5B92C927A411}">
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G68)))</xm:f>
+            <xm:f>$C$4="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G68:G72</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{33FCAECE-C126-4CD8-88BB-BA2CCA64EE6E}">
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G68)))</xm:f>
+            <xm:f>$C$7="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G68:G72</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A476B2B1-08FD-4830-9685-2B9301ABC130}">
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E68)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -5212,27 +5388,27 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E51</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{6F8E8C81-37C7-456F-AB40-6BB37581870D}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E52)))</xm:f>
-            <xm:f>$C$2="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E52:E55</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{7B8D20FF-1BC4-43A8-A3FB-313BCF9C61D9}">
+          <xm:sqref>E68:E71</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{9C271BA8-1993-4EBA-A422-018662325CBD}">
+            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C72)))</xm:f>
+            <xm:f>$C$16="Milestone"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C72</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{46D73D17-2031-4A48-B492-8BCD85146D14}">
             <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E72)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
@@ -5247,91 +5423,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>E72</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{4D7DB7FF-0A08-48FF-88DA-DD1F0BCC6135}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E67)))</xm:f>
-            <xm:f>$C$2="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{74FFE708-7A19-4167-8496-5B905FC265E4}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G68)))</xm:f>
-            <xm:f>$C$2="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G68:G71</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{AF0A3521-EB4E-400D-844A-5B92C927A411}">
-            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G68)))</xm:f>
-            <xm:f>$C$4="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G68:G71</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{33FCAECE-C126-4CD8-88BB-BA2CCA64EE6E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",G68)))</xm:f>
-            <xm:f>$C$7="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G68:G71</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A476B2B1-08FD-4830-9685-2B9301ABC130}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E68)))</xm:f>
-            <xm:f>$C$2="Milestone"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E68:E71</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Implemented a new movement algorithm
</commit_message>
<xml_diff>
--- a/dev/milestones.xlsx
+++ b/dev/milestones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="184">
   <si>
     <t>Core</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>Fade Popup out when specific object isn't active</t>
+  </si>
+  <si>
+    <t>Movement speed</t>
+  </si>
+  <si>
+    <t>Make units faster and implement game speed</t>
   </si>
 </sst>
 </file>
@@ -715,7 +721,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="113">
+  <dxfs count="112">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -788,16 +794,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2083,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3705,7 +3701,7 @@
         <v>41084</v>
       </c>
       <c r="G68" s="9" t="b">
-        <f>ISNUMBER(F68)</f>
+        <f t="shared" ref="G68:G73" si="22">ISNUMBER(F68)</f>
         <v>1</v>
       </c>
     </row>
@@ -3729,7 +3725,7 @@
         <v>41086</v>
       </c>
       <c r="G69" s="9" t="b">
-        <f>ISNUMBER(F69)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
@@ -3753,7 +3749,7 @@
         <v>41087</v>
       </c>
       <c r="G70" s="9" t="b">
-        <f>ISNUMBER(F70)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
@@ -3777,7 +3773,7 @@
         <v>41088</v>
       </c>
       <c r="G71" s="9" t="b">
-        <f>ISNUMBER(F71)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
@@ -3797,112 +3793,117 @@
       <c r="E72" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="F72" s="8">
+        <v>41089</v>
+      </c>
       <c r="G72" s="9" t="b">
-        <f>ISNUMBER(F72)</f>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="7"/>
+      <c r="E73" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G73" s="9" t="b">
-        <f>ISNUMBER(F73)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
-        <v>75</v>
+      <c r="A74" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="7"/>
       <c r="G74" s="9" t="b">
-        <f t="shared" ref="G74:G80" si="22">ISNUMBER(F74)</f>
+        <f>ISNUMBER(F74)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
-        <v>90</v>
+      <c r="A75" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E75" s="7"/>
       <c r="G75" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="G75:G81" si="23">ISNUMBER(F75)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E76" s="7"/>
       <c r="G76" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
-        <v>79</v>
+      <c r="A77" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="8"/>
+      <c r="E77" s="7"/>
       <c r="G77" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>27</v>
@@ -3912,16 +3913,16 @@
       </c>
       <c r="E78" s="8"/>
       <c r="G78" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>27</v>
@@ -3931,16 +3932,16 @@
       </c>
       <c r="E79" s="8"/>
       <c r="G79" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>27</v>
@@ -3950,79 +3951,80 @@
       </c>
       <c r="E80" s="8"/>
       <c r="G80" s="9" t="b">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="8"/>
+      <c r="G81" s="9" t="b">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="7"/>
-      <c r="G81" s="9" t="b">
-        <f t="shared" ref="G81" si="23">ISNUMBER(F81)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="7"/>
       <c r="G82" s="9" t="b">
-        <f>ISNUMBER(F82)</f>
+        <f t="shared" ref="G82" si="24">ISNUMBER(F82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D83" s="9"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="14"/>
+      <c r="A83" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="7"/>
       <c r="G83" s="9" t="b">
         <f>ISNUMBER(F83)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A84" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="9" t="b">
         <f>ISNUMBER(F84)</f>
         <v>0</v>
@@ -4030,10 +4032,10 @@
     </row>
     <row r="85" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>0</v>
@@ -4046,147 +4048,165 @@
         <v>0</v>
       </c>
     </row>
+    <row r="86" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G86" s="9" t="b">
+        <f>ISNUMBER(F86)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85">
-    <cfRule type="cellIs" dxfId="112" priority="161" operator="equal">
+  <conditionalFormatting sqref="G2:G20 H45:H49 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G74:G83 G85:G86">
+    <cfRule type="cellIs" dxfId="111" priority="161" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="162" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="110" priority="162" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85">
-    <cfRule type="cellIs" dxfId="110" priority="159" operator="equal">
+  <conditionalFormatting sqref="A3:D3 F3:G3 G4:G20 G22:G32 G35:G36 G49 G51 G39:G47 G56:G67 G74:G83 G85:G86">
+    <cfRule type="cellIs" dxfId="109" priority="159" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="109" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="133" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="134" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="107" priority="134" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="107" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="131" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="119" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="120" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="104" priority="120" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="104" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="117" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="103" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="80" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="81" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="101" priority="81" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="101" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="78" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="100" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="73" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="74" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="98" priority="74" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="98" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="71" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="97" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="62" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="63" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="95" priority="63" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="95" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="60" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G83">
-    <cfRule type="cellIs" dxfId="94" priority="46" operator="equal">
+  <conditionalFormatting sqref="G84">
+    <cfRule type="cellIs" dxfId="93" priority="46" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="47" operator="containsText" text="FALSCH">
-      <formula>NOT(ISERROR(SEARCH("FALSCH",G83)))</formula>
+    <cfRule type="containsText" dxfId="92" priority="47" operator="containsText" text="FALSCH">
+      <formula>NOT(ISERROR(SEARCH("FALSCH",G84)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G83">
-    <cfRule type="cellIs" dxfId="92" priority="44" operator="equal">
+  <conditionalFormatting sqref="G84">
+    <cfRule type="cellIs" dxfId="91" priority="44" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="91" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="38" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="39" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="89" priority="39" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="89" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="36" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="88" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="31" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="86" priority="31" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="cellIs" dxfId="86" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="28" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="85" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="25" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="83" priority="25" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G55">
-    <cfRule type="cellIs" dxfId="83" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G72">
-    <cfRule type="cellIs" dxfId="82" priority="8" operator="equal">
+  <conditionalFormatting sqref="G68:G73">
+    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="FALSCH">
+    <cfRule type="containsText" dxfId="80" priority="9" operator="containsText" text="FALSCH">
       <formula>NOT(ISERROR(SEARCH("FALSCH",G68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68:G72">
-    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+  <conditionalFormatting sqref="G68:G73">
+    <cfRule type="cellIs" dxfId="79" priority="6" operator="equal">
       <formula>$C$3="Milestone"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4215,7 +4235,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E81:E82 E63:E65 E75:E76 G56:G67 G73:G82 G84:G85</xm:sqref>
+          <xm:sqref>A2:G2 E3:E13 E15:E20 G3:G20 G22:G32 E27:E32 G35:G36 E35:E36 E44:E46 E39:E42 G49 G51 G39:G47 E82:E83 E63:E65 E76:E77 G56:G67 G74:G83 G85:G86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="158" operator="containsText" id="{51168458-9BAB-408F-B327-6A9DB8979B23}">
@@ -4232,7 +4252,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G73:G82 G84:G85</xm:sqref>
+          <xm:sqref>A4:D4 F4:G4 G5:G20 G22:G32 G35:G36 D50 G49 G51 G39:G47 G56:G67 G74:G83 G85:G86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="156" operator="containsText" id="{D3E5AAE4-E477-4153-B088-7C3C62450C49}">
@@ -4249,7 +4269,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G73:G82 G84:G85</xm:sqref>
+          <xm:sqref>F7 A7:D7 G5 G8:G20 A14:D14 A21:D21 A34:D34 A47:D47 A66:D66 G22:G32 G35:G36 G51 G39:G47 G56:G67 G74:G83 G85:G86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="143" operator="containsText" id="{757235BB-F1BF-491F-8FD2-93B47182FE41}">
@@ -4300,7 +4320,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C81</xm:sqref>
+          <xm:sqref>G6:G7 C15:C16 C18:C19 C43 G49 C59 C82</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="132" operator="containsText" id="{48BB4CEB-160E-479C-AD26-E46B029C5254}">
@@ -4593,7 +4613,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="90" operator="containsText" id="{494BDCB2-477F-4CCA-8E56-B54621BD2FC3}">
-            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C76)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$16="Milestone",C77)))</xm:f>
             <xm:f>$C$16="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4606,7 +4626,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C76</xm:sqref>
+          <xm:sqref>C77</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="82" operator="containsText" id="{E4DC5AB8-267C-41A9-804E-ED83F72EC3B3}">
@@ -4899,7 +4919,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="45" operator="containsText" id="{F6528D32-36D9-4F3D-BCB9-7BB591B2340A}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G83)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",G84)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4912,11 +4932,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G83</xm:sqref>
+          <xm:sqref>G84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="43" operator="containsText" id="{4B016956-2296-4401-915A-F72B0EAA9908}">
-            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G83)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$4="Milestone",G84)))</xm:f>
             <xm:f>$C$4="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4929,11 +4949,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G83</xm:sqref>
+          <xm:sqref>G84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="42" operator="containsText" id="{1D88AD4A-6D83-4A08-BCE8-C66B966B0073}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A83)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",A84)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4946,11 +4966,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A83:D83 G83</xm:sqref>
+          <xm:sqref>A84:D84 G84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="41" operator="containsText" id="{9D7F58D5-CCAB-4E73-B86A-50D80AAAAC5E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E83)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E84)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4963,11 +4983,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E83</xm:sqref>
+          <xm:sqref>E84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="40" operator="containsText" id="{C4DFE680-2DE8-4DC5-9900-C8462125156E}">
-            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F83)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$7="Milestone",F84)))</xm:f>
             <xm:f>$C$7="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -4980,7 +5000,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F83</xm:sqref>
+          <xm:sqref>F84</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="37" operator="containsText" id="{992FC9B3-D313-4572-8AB6-63618C6AE8A6}">
@@ -5205,7 +5225,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="17" operator="containsText" id="{4C3F2991-D8EC-410C-9B0B-CF4EC4549A8D}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E74)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E75)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -5218,7 +5238,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E74</xm:sqref>
+          <xm:sqref>E75</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="16" operator="containsText" id="{B92B02FA-3804-4C2D-8DFB-01196540492A}">
@@ -5290,7 +5310,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="12" operator="containsText" id="{7B8D20FF-1BC4-43A8-A3FB-313BCF9C61D9}">
-            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E73)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$2="Milestone",E74)))</xm:f>
             <xm:f>$C$2="Milestone"</xm:f>
             <x14:dxf>
               <font>
@@ -5303,7 +5323,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E73</xm:sqref>
+          <xm:sqref>E74</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="10" operator="containsText" id="{4D7DB7FF-0A08-48FF-88DA-DD1F0BCC6135}">
@@ -5337,7 +5357,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G72</xm:sqref>
+          <xm:sqref>G68:G73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="5" operator="containsText" id="{AF0A3521-EB4E-400D-844A-5B92C927A411}">
@@ -5354,7 +5374,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G72</xm:sqref>
+          <xm:sqref>G68:G73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{33FCAECE-C126-4CD8-88BB-BA2CCA64EE6E}">
@@ -5371,7 +5391,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G68:G72</xm:sqref>
+          <xm:sqref>G68:G73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A476B2B1-08FD-4830-9685-2B9301ABC130}">
@@ -5422,7 +5442,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E72</xm:sqref>
+          <xm:sqref>E72:E73</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>